<commit_message>
Se añade el modo buscador (test)
</commit_message>
<xml_diff>
--- a/Agil - Copia de Preguntas_Examen.xlsx
+++ b/Agil - Copia de Preguntas_Examen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jormart\Desktop\miscellaneous\safe-trainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B092D-C346-4465-92CC-F4E18F1F695C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8A9A00-5E46-4675-9C53-C296F2F11E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3692,11 +3692,10 @@
     <t>To enable releasing functionality on demand to meet business needs</t>
   </si>
   <si>
-    <t>Customer collaboration over contract negotiation;
-Individual interactions over processes and tools</t>
-  </si>
-  <si>
-    <t>External; Customers</t>
+    <t>External;Customers</t>
+  </si>
+  <si>
+    <t>Customer collaboration over contract negotiation;Individual interactions over processes and tools</t>
   </si>
 </sst>
 </file>
@@ -4064,8 +4063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="D243" sqref="D243"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4973,7 +4972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4984,7 +4983,7 @@
         <v>139</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -8844,7 +8843,7 @@
         <v>677</v>
       </c>
       <c r="D239" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E239">
         <v>0</v>
@@ -10395,6 +10394,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Fichero de Preguntas - Corrección
</commit_message>
<xml_diff>
--- a/Agil - Copia de Preguntas_Examen.xlsx
+++ b/Agil - Copia de Preguntas_Examen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jormart\Desktop\miscellaneous\safe-trainer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GBHRZRL\Desktop\SRC\safe-trainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA27CF7-EACC-4B3B-8349-DF5AE8022C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF6E61-9BBF-4F55-BD9C-B0B32882FB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2475,9 +2475,6 @@
 Working software is the primary measure of progress</t>
   </si>
   <si>
-    <t>Responding to change</t>
-  </si>
-  <si>
     <t>What brings structure to analysis and decision making around Epics?</t>
   </si>
   <si>
@@ -3696,6 +3693,9 @@
   </si>
   <si>
     <t>The Product Manager makes weekly visits to a customer's site. Which two Agile Manifesto Values support this behavior? (Choose two)</t>
+  </si>
+  <si>
+    <t>Responding to change over following a plan</t>
   </si>
 </sst>
 </file>
@@ -4063,17 +4063,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="165.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="165.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4973,18 +4973,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C46" t="s">
         <v>138</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4993,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -7213,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -7353,15 +7353,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165" t="s">
+        <v>896</v>
+      </c>
+      <c r="C165" t="s">
         <v>897</v>
-      </c>
-      <c r="C165" t="s">
-        <v>898</v>
       </c>
       <c r="D165" t="s">
         <v>485</v>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>170</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>171</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>172</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>173</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>174</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>175</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>176</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>177</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>178</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>179</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>182</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>185</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>186</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>551</v>
       </c>
       <c r="D189" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E189">
         <v>0</v>
@@ -7853,7 +7853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>189</v>
       </c>
@@ -7861,11 +7861,11 @@
         <v>552</v>
       </c>
       <c r="C190" t="s">
+        <v>899</v>
+      </c>
+      <c r="D190" t="s">
         <v>900</v>
       </c>
-      <c r="D190" t="s">
-        <v>901</v>
-      </c>
       <c r="E190">
         <v>0</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>190</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>555</v>
       </c>
       <c r="D191" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E191">
         <v>0</v>
@@ -7893,7 +7893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>191</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>192</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>193</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>563</v>
       </c>
       <c r="D194" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E194">
         <v>0</v>
@@ -7953,7 +7953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>194</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>195</v>
       </c>
@@ -7993,18 +7993,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C197" t="s">
         <v>570</v>
       </c>
       <c r="D197" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E197">
         <v>0</v>
@@ -8013,7 +8013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>197</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>198</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>574</v>
       </c>
       <c r="D199" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E199">
         <v>0</v>
@@ -8053,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>199</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>576</v>
       </c>
       <c r="D200" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E200">
         <v>0</v>
@@ -8073,7 +8073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>200</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>201</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>202</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>203</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>204</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>205</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>206</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>207</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>208</v>
       </c>
@@ -8253,7 +8253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>209</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>210</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>211</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>606</v>
       </c>
       <c r="D212" t="s">
-        <v>607</v>
+        <v>910</v>
       </c>
       <c r="E212">
         <v>0</v>
@@ -8313,15 +8313,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>212</v>
       </c>
       <c r="B213" t="s">
+        <v>607</v>
+      </c>
+      <c r="C213" t="s">
         <v>608</v>
-      </c>
-      <c r="C213" t="s">
-        <v>609</v>
       </c>
       <c r="D213" t="s">
         <v>553</v>
@@ -8333,12 +8333,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C214" t="s">
         <v>43</v>
@@ -8353,19 +8353,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215" t="s">
+        <v>610</v>
+      </c>
+      <c r="C215" t="s">
         <v>611</v>
       </c>
-      <c r="C215" t="s">
+      <c r="D215" t="s">
         <v>612</v>
       </c>
-      <c r="D215" t="s">
-        <v>613</v>
-      </c>
       <c r="E215">
         <v>0</v>
       </c>
@@ -8373,19 +8373,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>215</v>
       </c>
       <c r="B216" t="s">
+        <v>613</v>
+      </c>
+      <c r="C216" t="s">
         <v>614</v>
       </c>
-      <c r="C216" t="s">
+      <c r="D216" t="s">
         <v>615</v>
       </c>
-      <c r="D216" t="s">
-        <v>616</v>
-      </c>
       <c r="E216">
         <v>0</v>
       </c>
@@ -8393,19 +8393,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
+        <v>616</v>
+      </c>
+      <c r="C217" t="s">
         <v>617</v>
       </c>
-      <c r="C217" t="s">
+      <c r="D217" t="s">
         <v>618</v>
       </c>
-      <c r="D217" t="s">
-        <v>619</v>
-      </c>
       <c r="E217">
         <v>0</v>
       </c>
@@ -8413,19 +8413,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218" t="s">
+        <v>619</v>
+      </c>
+      <c r="C218" t="s">
         <v>620</v>
       </c>
-      <c r="C218" t="s">
+      <c r="D218" t="s">
         <v>621</v>
       </c>
-      <c r="D218" t="s">
-        <v>622</v>
-      </c>
       <c r="E218">
         <v>0</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>218</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>267</v>
       </c>
       <c r="C219" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D219" t="s">
         <v>269</v>
@@ -8453,19 +8453,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>219</v>
       </c>
       <c r="B220" t="s">
+        <v>623</v>
+      </c>
+      <c r="C220" t="s">
         <v>624</v>
       </c>
-      <c r="C220" t="s">
+      <c r="D220" t="s">
         <v>625</v>
       </c>
-      <c r="D220" t="s">
-        <v>626</v>
-      </c>
       <c r="E220">
         <v>0</v>
       </c>
@@ -8473,19 +8473,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>220</v>
       </c>
       <c r="B221" t="s">
+        <v>626</v>
+      </c>
+      <c r="C221" t="s">
         <v>627</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>628</v>
       </c>
-      <c r="D221" t="s">
-        <v>629</v>
-      </c>
       <c r="E221">
         <v>0</v>
       </c>
@@ -8493,15 +8493,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>221</v>
       </c>
       <c r="B222" t="s">
+        <v>629</v>
+      </c>
+      <c r="C222" t="s">
         <v>630</v>
-      </c>
-      <c r="C222" t="s">
-        <v>631</v>
       </c>
       <c r="D222" t="s">
         <v>375</v>
@@ -8513,19 +8513,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>222</v>
       </c>
       <c r="B223" t="s">
+        <v>631</v>
+      </c>
+      <c r="C223" t="s">
         <v>632</v>
       </c>
-      <c r="C223" t="s">
+      <c r="D223" t="s">
         <v>633</v>
       </c>
-      <c r="D223" t="s">
-        <v>634</v>
-      </c>
       <c r="E223">
         <v>0</v>
       </c>
@@ -8533,18 +8533,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C224" t="s">
         <v>197</v>
       </c>
       <c r="D224" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E224">
         <v>0</v>
@@ -8553,19 +8553,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225" t="s">
+        <v>636</v>
+      </c>
+      <c r="C225" t="s">
         <v>637</v>
       </c>
-      <c r="C225" t="s">
+      <c r="D225" t="s">
         <v>638</v>
       </c>
-      <c r="D225" t="s">
-        <v>639</v>
-      </c>
       <c r="E225">
         <v>0</v>
       </c>
@@ -8573,19 +8573,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>225</v>
       </c>
       <c r="B226" t="s">
+        <v>639</v>
+      </c>
+      <c r="C226" t="s">
         <v>640</v>
       </c>
-      <c r="C226" t="s">
+      <c r="D226" t="s">
         <v>641</v>
       </c>
-      <c r="D226" t="s">
-        <v>642</v>
-      </c>
       <c r="E226">
         <v>0</v>
       </c>
@@ -8593,19 +8593,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>226</v>
       </c>
       <c r="B227" t="s">
+        <v>642</v>
+      </c>
+      <c r="C227" t="s">
         <v>643</v>
       </c>
-      <c r="C227" t="s">
+      <c r="D227" t="s">
         <v>644</v>
       </c>
-      <c r="D227" t="s">
-        <v>645</v>
-      </c>
       <c r="E227">
         <v>0</v>
       </c>
@@ -8613,18 +8613,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>227</v>
       </c>
       <c r="B228" t="s">
+        <v>645</v>
+      </c>
+      <c r="C228" t="s">
         <v>646</v>
       </c>
-      <c r="C228" t="s">
-        <v>647</v>
-      </c>
       <c r="D228" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E228">
         <v>0</v>
@@ -8633,19 +8633,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>228</v>
       </c>
       <c r="B229" t="s">
+        <v>647</v>
+      </c>
+      <c r="C229" t="s">
         <v>648</v>
       </c>
-      <c r="C229" t="s">
+      <c r="D229" t="s">
         <v>649</v>
       </c>
-      <c r="D229" t="s">
-        <v>650</v>
-      </c>
       <c r="E229">
         <v>0</v>
       </c>
@@ -8653,19 +8653,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>229</v>
       </c>
       <c r="B230" t="s">
+        <v>650</v>
+      </c>
+      <c r="C230" t="s">
         <v>651</v>
       </c>
-      <c r="C230" t="s">
+      <c r="D230" t="s">
         <v>652</v>
       </c>
-      <c r="D230" t="s">
-        <v>653</v>
-      </c>
       <c r="E230">
         <v>0</v>
       </c>
@@ -8673,19 +8673,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>230</v>
       </c>
       <c r="B231" t="s">
+        <v>653</v>
+      </c>
+      <c r="C231" t="s">
         <v>654</v>
       </c>
-      <c r="C231" t="s">
+      <c r="D231" t="s">
         <v>655</v>
       </c>
-      <c r="D231" t="s">
-        <v>656</v>
-      </c>
       <c r="E231">
         <v>0</v>
       </c>
@@ -8693,19 +8693,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>231</v>
       </c>
       <c r="B232" t="s">
+        <v>656</v>
+      </c>
+      <c r="C232" t="s">
         <v>657</v>
       </c>
-      <c r="C232" t="s">
+      <c r="D232" t="s">
         <v>658</v>
       </c>
-      <c r="D232" t="s">
-        <v>659</v>
-      </c>
       <c r="E232">
         <v>0</v>
       </c>
@@ -8713,19 +8713,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>232</v>
       </c>
       <c r="B233" t="s">
+        <v>659</v>
+      </c>
+      <c r="C233" t="s">
         <v>660</v>
       </c>
-      <c r="C233" t="s">
+      <c r="D233" t="s">
         <v>661</v>
       </c>
-      <c r="D233" t="s">
-        <v>662</v>
-      </c>
       <c r="E233">
         <v>0</v>
       </c>
@@ -8733,12 +8733,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C234" t="s">
         <v>356</v>
@@ -8753,15 +8753,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>234</v>
       </c>
       <c r="B235" t="s">
+        <v>663</v>
+      </c>
+      <c r="C235" t="s">
         <v>664</v>
-      </c>
-      <c r="C235" t="s">
-        <v>665</v>
       </c>
       <c r="D235" t="s">
         <v>165</v>
@@ -8773,19 +8773,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>235</v>
       </c>
       <c r="B236" t="s">
+        <v>665</v>
+      </c>
+      <c r="C236" t="s">
         <v>666</v>
       </c>
-      <c r="C236" t="s">
+      <c r="D236" t="s">
         <v>667</v>
       </c>
-      <c r="D236" t="s">
-        <v>668</v>
-      </c>
       <c r="E236">
         <v>0</v>
       </c>
@@ -8793,19 +8793,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>236</v>
       </c>
       <c r="B237" t="s">
+        <v>668</v>
+      </c>
+      <c r="C237" t="s">
         <v>669</v>
       </c>
-      <c r="C237" t="s">
+      <c r="D237" t="s">
         <v>670</v>
       </c>
-      <c r="D237" t="s">
-        <v>671</v>
-      </c>
       <c r="E237">
         <v>0</v>
       </c>
@@ -8813,19 +8813,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>237</v>
       </c>
       <c r="B238" t="s">
+        <v>671</v>
+      </c>
+      <c r="C238" t="s">
         <v>672</v>
       </c>
-      <c r="C238" t="s">
+      <c r="D238" t="s">
         <v>673</v>
       </c>
-      <c r="D238" t="s">
-        <v>674</v>
-      </c>
       <c r="E238">
         <v>0</v>
       </c>
@@ -8833,18 +8833,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>238</v>
       </c>
       <c r="B239" t="s">
+        <v>674</v>
+      </c>
+      <c r="C239" t="s">
         <v>675</v>
       </c>
-      <c r="C239" t="s">
-        <v>676</v>
-      </c>
       <c r="D239" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E239">
         <v>0</v>
@@ -8853,19 +8853,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>239</v>
       </c>
       <c r="B240" t="s">
+        <v>676</v>
+      </c>
+      <c r="C240" t="s">
         <v>677</v>
       </c>
-      <c r="C240" t="s">
+      <c r="D240" t="s">
         <v>678</v>
       </c>
-      <c r="D240" t="s">
-        <v>679</v>
-      </c>
       <c r="E240">
         <v>0</v>
       </c>
@@ -8873,19 +8873,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>240</v>
       </c>
       <c r="B241" t="s">
+        <v>679</v>
+      </c>
+      <c r="C241" t="s">
         <v>680</v>
       </c>
-      <c r="C241" t="s">
+      <c r="D241" t="s">
         <v>681</v>
       </c>
-      <c r="D241" t="s">
-        <v>682</v>
-      </c>
       <c r="E241">
         <v>0</v>
       </c>
@@ -8893,19 +8893,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" t="s">
+        <v>682</v>
+      </c>
+      <c r="C242" t="s">
         <v>683</v>
       </c>
-      <c r="C242" t="s">
+      <c r="D242" t="s">
         <v>684</v>
       </c>
-      <c r="D242" t="s">
-        <v>685</v>
-      </c>
       <c r="E242">
         <v>0</v>
       </c>
@@ -8913,19 +8913,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>242</v>
       </c>
       <c r="B243" t="s">
+        <v>685</v>
+      </c>
+      <c r="C243" t="s">
         <v>686</v>
       </c>
-      <c r="C243" t="s">
+      <c r="D243" t="s">
         <v>687</v>
       </c>
-      <c r="D243" t="s">
-        <v>688</v>
-      </c>
       <c r="E243">
         <v>0</v>
       </c>
@@ -8933,19 +8933,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>243</v>
       </c>
       <c r="B244" t="s">
+        <v>688</v>
+      </c>
+      <c r="C244" t="s">
         <v>689</v>
       </c>
-      <c r="C244" t="s">
+      <c r="D244" t="s">
         <v>690</v>
       </c>
-      <c r="D244" t="s">
-        <v>691</v>
-      </c>
       <c r="E244">
         <v>0</v>
       </c>
@@ -8953,19 +8953,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>244</v>
       </c>
       <c r="B245" t="s">
+        <v>691</v>
+      </c>
+      <c r="C245" t="s">
         <v>692</v>
       </c>
-      <c r="C245" t="s">
+      <c r="D245" t="s">
         <v>693</v>
       </c>
-      <c r="D245" t="s">
-        <v>694</v>
-      </c>
       <c r="E245">
         <v>0</v>
       </c>
@@ -8973,19 +8973,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>245</v>
       </c>
       <c r="B246" t="s">
+        <v>694</v>
+      </c>
+      <c r="C246" t="s">
         <v>695</v>
       </c>
-      <c r="C246" t="s">
+      <c r="D246" t="s">
         <v>696</v>
       </c>
-      <c r="D246" t="s">
-        <v>697</v>
-      </c>
       <c r="E246">
         <v>0</v>
       </c>
@@ -8993,19 +8993,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>246</v>
       </c>
       <c r="B247" t="s">
+        <v>697</v>
+      </c>
+      <c r="C247" t="s">
         <v>698</v>
       </c>
-      <c r="C247" t="s">
+      <c r="D247" t="s">
         <v>699</v>
       </c>
-      <c r="D247" t="s">
-        <v>700</v>
-      </c>
       <c r="E247">
         <v>0</v>
       </c>
@@ -9013,19 +9013,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>247</v>
       </c>
       <c r="B248" t="s">
+        <v>700</v>
+      </c>
+      <c r="C248" t="s">
         <v>701</v>
       </c>
-      <c r="C248" t="s">
+      <c r="D248" t="s">
         <v>702</v>
       </c>
-      <c r="D248" t="s">
-        <v>703</v>
-      </c>
       <c r="E248">
         <v>0</v>
       </c>
@@ -9033,19 +9033,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>248</v>
       </c>
       <c r="B249" t="s">
+        <v>703</v>
+      </c>
+      <c r="C249" t="s">
         <v>704</v>
       </c>
-      <c r="C249" t="s">
+      <c r="D249" t="s">
         <v>705</v>
       </c>
-      <c r="D249" t="s">
-        <v>706</v>
-      </c>
       <c r="E249">
         <v>0</v>
       </c>
@@ -9053,19 +9053,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>249</v>
       </c>
       <c r="B250" t="s">
+        <v>706</v>
+      </c>
+      <c r="C250" t="s">
         <v>707</v>
       </c>
-      <c r="C250" t="s">
+      <c r="D250" t="s">
         <v>708</v>
       </c>
-      <c r="D250" t="s">
-        <v>709</v>
-      </c>
       <c r="E250">
         <v>0</v>
       </c>
@@ -9073,19 +9073,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>250</v>
       </c>
       <c r="B251" t="s">
+        <v>709</v>
+      </c>
+      <c r="C251" t="s">
         <v>710</v>
       </c>
-      <c r="C251" t="s">
+      <c r="D251" t="s">
         <v>711</v>
       </c>
-      <c r="D251" t="s">
-        <v>712</v>
-      </c>
       <c r="E251">
         <v>0</v>
       </c>
@@ -9093,19 +9093,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>251</v>
       </c>
       <c r="B252" t="s">
+        <v>712</v>
+      </c>
+      <c r="C252" t="s">
         <v>713</v>
       </c>
-      <c r="C252" t="s">
+      <c r="D252" t="s">
         <v>714</v>
       </c>
-      <c r="D252" t="s">
-        <v>715</v>
-      </c>
       <c r="E252">
         <v>0</v>
       </c>
@@ -9113,19 +9113,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>252</v>
       </c>
       <c r="B253" t="s">
+        <v>715</v>
+      </c>
+      <c r="C253" t="s">
         <v>716</v>
       </c>
-      <c r="C253" t="s">
+      <c r="D253" t="s">
         <v>717</v>
       </c>
-      <c r="D253" t="s">
-        <v>718</v>
-      </c>
       <c r="E253">
         <v>0</v>
       </c>
@@ -9133,19 +9133,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>253</v>
       </c>
       <c r="B254" t="s">
+        <v>718</v>
+      </c>
+      <c r="C254" t="s">
         <v>719</v>
       </c>
-      <c r="C254" t="s">
+      <c r="D254" t="s">
         <v>720</v>
       </c>
-      <c r="D254" t="s">
-        <v>721</v>
-      </c>
       <c r="E254">
         <v>0</v>
       </c>
@@ -9153,19 +9153,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>254</v>
       </c>
       <c r="B255" t="s">
+        <v>721</v>
+      </c>
+      <c r="C255" t="s">
         <v>722</v>
       </c>
-      <c r="C255" t="s">
+      <c r="D255" t="s">
         <v>723</v>
       </c>
-      <c r="D255" t="s">
-        <v>724</v>
-      </c>
       <c r="E255">
         <v>0</v>
       </c>
@@ -9173,19 +9173,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>255</v>
       </c>
       <c r="B256" t="s">
+        <v>724</v>
+      </c>
+      <c r="C256" t="s">
         <v>725</v>
       </c>
-      <c r="C256" t="s">
+      <c r="D256" t="s">
         <v>726</v>
       </c>
-      <c r="D256" t="s">
-        <v>727</v>
-      </c>
       <c r="E256">
         <v>0</v>
       </c>
@@ -9193,19 +9193,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>256</v>
       </c>
       <c r="B257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C257" t="s">
         <v>728</v>
       </c>
-      <c r="C257" t="s">
+      <c r="D257" t="s">
         <v>729</v>
       </c>
-      <c r="D257" t="s">
-        <v>730</v>
-      </c>
       <c r="E257">
         <v>0</v>
       </c>
@@ -9213,19 +9213,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>257</v>
       </c>
       <c r="B258" t="s">
+        <v>730</v>
+      </c>
+      <c r="C258" t="s">
         <v>731</v>
       </c>
-      <c r="C258" t="s">
+      <c r="D258" t="s">
         <v>732</v>
       </c>
-      <c r="D258" t="s">
-        <v>733</v>
-      </c>
       <c r="E258">
         <v>0</v>
       </c>
@@ -9233,19 +9233,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>258</v>
       </c>
       <c r="B259" t="s">
+        <v>733</v>
+      </c>
+      <c r="C259" t="s">
         <v>734</v>
       </c>
-      <c r="C259" t="s">
+      <c r="D259" t="s">
         <v>735</v>
       </c>
-      <c r="D259" t="s">
-        <v>736</v>
-      </c>
       <c r="E259">
         <v>0</v>
       </c>
@@ -9253,19 +9253,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>259</v>
       </c>
       <c r="B260" t="s">
+        <v>736</v>
+      </c>
+      <c r="C260" t="s">
         <v>737</v>
       </c>
-      <c r="C260" t="s">
+      <c r="D260" t="s">
         <v>738</v>
       </c>
-      <c r="D260" t="s">
-        <v>739</v>
-      </c>
       <c r="E260">
         <v>0</v>
       </c>
@@ -9273,19 +9273,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>260</v>
       </c>
       <c r="B261" t="s">
+        <v>739</v>
+      </c>
+      <c r="C261" t="s">
         <v>740</v>
       </c>
-      <c r="C261" t="s">
+      <c r="D261" t="s">
         <v>741</v>
       </c>
-      <c r="D261" t="s">
-        <v>742</v>
-      </c>
       <c r="E261">
         <v>0</v>
       </c>
@@ -9293,15 +9293,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>261</v>
       </c>
       <c r="B262" t="s">
+        <v>742</v>
+      </c>
+      <c r="C262" t="s">
         <v>743</v>
-      </c>
-      <c r="C262" t="s">
-        <v>744</v>
       </c>
       <c r="D262" t="s">
         <v>561</v>
@@ -9313,19 +9313,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>262</v>
       </c>
       <c r="B263" t="s">
+        <v>744</v>
+      </c>
+      <c r="C263" t="s">
         <v>745</v>
       </c>
-      <c r="C263" t="s">
+      <c r="D263" t="s">
         <v>746</v>
       </c>
-      <c r="D263" t="s">
-        <v>747</v>
-      </c>
       <c r="E263">
         <v>0</v>
       </c>
@@ -9333,19 +9333,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>263</v>
       </c>
       <c r="B264" t="s">
+        <v>747</v>
+      </c>
+      <c r="C264" t="s">
         <v>748</v>
       </c>
-      <c r="C264" t="s">
+      <c r="D264" t="s">
         <v>749</v>
       </c>
-      <c r="D264" t="s">
-        <v>750</v>
-      </c>
       <c r="E264">
         <v>0</v>
       </c>
@@ -9353,19 +9353,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>264</v>
       </c>
       <c r="B265" t="s">
+        <v>750</v>
+      </c>
+      <c r="C265" t="s">
         <v>751</v>
       </c>
-      <c r="C265" t="s">
+      <c r="D265" t="s">
         <v>752</v>
       </c>
-      <c r="D265" t="s">
-        <v>753</v>
-      </c>
       <c r="E265">
         <v>0</v>
       </c>
@@ -9373,19 +9373,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>265</v>
       </c>
       <c r="B266" t="s">
+        <v>753</v>
+      </c>
+      <c r="C266" t="s">
         <v>754</v>
       </c>
-      <c r="C266" t="s">
+      <c r="D266" t="s">
         <v>755</v>
       </c>
-      <c r="D266" t="s">
-        <v>756</v>
-      </c>
       <c r="E266">
         <v>0</v>
       </c>
@@ -9393,19 +9393,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>266</v>
       </c>
       <c r="B267" t="s">
+        <v>756</v>
+      </c>
+      <c r="C267" t="s">
         <v>757</v>
       </c>
-      <c r="C267" t="s">
+      <c r="D267" t="s">
         <v>758</v>
       </c>
-      <c r="D267" t="s">
-        <v>759</v>
-      </c>
       <c r="E267">
         <v>0</v>
       </c>
@@ -9413,19 +9413,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>267</v>
       </c>
       <c r="B268" t="s">
+        <v>759</v>
+      </c>
+      <c r="C268" t="s">
         <v>760</v>
       </c>
-      <c r="C268" t="s">
+      <c r="D268" t="s">
         <v>761</v>
       </c>
-      <c r="D268" t="s">
-        <v>762</v>
-      </c>
       <c r="E268">
         <v>0</v>
       </c>
@@ -9433,15 +9433,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>268</v>
       </c>
       <c r="B269" t="s">
+        <v>762</v>
+      </c>
+      <c r="C269" t="s">
         <v>763</v>
-      </c>
-      <c r="C269" t="s">
-        <v>764</v>
       </c>
       <c r="D269" t="s">
         <v>507</v>
@@ -9453,19 +9453,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>269</v>
       </c>
       <c r="B270" t="s">
+        <v>764</v>
+      </c>
+      <c r="C270" t="s">
         <v>765</v>
       </c>
-      <c r="C270" t="s">
+      <c r="D270" t="s">
         <v>766</v>
       </c>
-      <c r="D270" t="s">
-        <v>767</v>
-      </c>
       <c r="E270">
         <v>0</v>
       </c>
@@ -9473,19 +9473,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>270</v>
       </c>
       <c r="B271" t="s">
+        <v>767</v>
+      </c>
+      <c r="C271" t="s">
         <v>768</v>
       </c>
-      <c r="C271" t="s">
+      <c r="D271" t="s">
         <v>769</v>
       </c>
-      <c r="D271" t="s">
-        <v>770</v>
-      </c>
       <c r="E271">
         <v>0</v>
       </c>
@@ -9493,19 +9493,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>271</v>
       </c>
       <c r="B272" t="s">
+        <v>770</v>
+      </c>
+      <c r="C272" t="s">
         <v>771</v>
       </c>
-      <c r="C272" t="s">
+      <c r="D272" t="s">
         <v>772</v>
       </c>
-      <c r="D272" t="s">
-        <v>773</v>
-      </c>
       <c r="E272">
         <v>0</v>
       </c>
@@ -9513,19 +9513,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>272</v>
       </c>
       <c r="B273" t="s">
+        <v>773</v>
+      </c>
+      <c r="C273" t="s">
         <v>774</v>
       </c>
-      <c r="C273" t="s">
+      <c r="D273" t="s">
         <v>775</v>
       </c>
-      <c r="D273" t="s">
-        <v>776</v>
-      </c>
       <c r="E273">
         <v>0</v>
       </c>
@@ -9533,19 +9533,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>273</v>
       </c>
       <c r="B274" t="s">
+        <v>776</v>
+      </c>
+      <c r="C274" t="s">
         <v>777</v>
       </c>
-      <c r="C274" t="s">
+      <c r="D274" t="s">
         <v>778</v>
       </c>
-      <c r="D274" t="s">
-        <v>779</v>
-      </c>
       <c r="E274">
         <v>0</v>
       </c>
@@ -9553,19 +9553,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>274</v>
       </c>
       <c r="B275" t="s">
+        <v>779</v>
+      </c>
+      <c r="C275" t="s">
         <v>780</v>
       </c>
-      <c r="C275" t="s">
+      <c r="D275" t="s">
         <v>781</v>
       </c>
-      <c r="D275" t="s">
-        <v>782</v>
-      </c>
       <c r="E275">
         <v>0</v>
       </c>
@@ -9573,19 +9573,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>275</v>
       </c>
       <c r="B276" t="s">
+        <v>782</v>
+      </c>
+      <c r="C276" t="s">
         <v>783</v>
       </c>
-      <c r="C276" t="s">
+      <c r="D276" t="s">
         <v>784</v>
       </c>
-      <c r="D276" t="s">
-        <v>785</v>
-      </c>
       <c r="E276">
         <v>0</v>
       </c>
@@ -9593,19 +9593,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>276</v>
       </c>
       <c r="B277" t="s">
+        <v>785</v>
+      </c>
+      <c r="C277" t="s">
         <v>786</v>
       </c>
-      <c r="C277" t="s">
+      <c r="D277" t="s">
         <v>787</v>
       </c>
-      <c r="D277" t="s">
-        <v>788</v>
-      </c>
       <c r="E277">
         <v>0</v>
       </c>
@@ -9613,19 +9613,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C278" t="s">
+        <v>788</v>
+      </c>
+      <c r="D278" t="s">
         <v>789</v>
       </c>
-      <c r="D278" t="s">
-        <v>790</v>
-      </c>
       <c r="E278">
         <v>0</v>
       </c>
@@ -9633,15 +9633,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>278</v>
       </c>
       <c r="B279" t="s">
+        <v>790</v>
+      </c>
+      <c r="C279" t="s">
         <v>791</v>
-      </c>
-      <c r="C279" t="s">
-        <v>792</v>
       </c>
       <c r="D279" t="s">
         <v>455</v>
@@ -9653,19 +9653,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>279</v>
       </c>
       <c r="B280" t="s">
+        <v>792</v>
+      </c>
+      <c r="C280" t="s">
         <v>793</v>
       </c>
-      <c r="C280" t="s">
+      <c r="D280" t="s">
         <v>794</v>
       </c>
-      <c r="D280" t="s">
-        <v>795</v>
-      </c>
       <c r="E280">
         <v>0</v>
       </c>
@@ -9673,19 +9673,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>280</v>
       </c>
       <c r="B281" t="s">
+        <v>795</v>
+      </c>
+      <c r="C281" t="s">
         <v>796</v>
       </c>
-      <c r="C281" t="s">
+      <c r="D281" t="s">
         <v>797</v>
       </c>
-      <c r="D281" t="s">
-        <v>798</v>
-      </c>
       <c r="E281">
         <v>0</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>281</v>
       </c>
@@ -9701,11 +9701,11 @@
         <v>27</v>
       </c>
       <c r="C282" t="s">
+        <v>798</v>
+      </c>
+      <c r="D282" t="s">
         <v>799</v>
       </c>
-      <c r="D282" t="s">
-        <v>800</v>
-      </c>
       <c r="E282">
         <v>0</v>
       </c>
@@ -9713,19 +9713,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>282</v>
       </c>
       <c r="B283" t="s">
+        <v>800</v>
+      </c>
+      <c r="C283" t="s">
         <v>801</v>
       </c>
-      <c r="C283" t="s">
+      <c r="D283" t="s">
         <v>802</v>
       </c>
-      <c r="D283" t="s">
-        <v>803</v>
-      </c>
       <c r="E283">
         <v>0</v>
       </c>
@@ -9733,19 +9733,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>283</v>
       </c>
       <c r="B284" t="s">
+        <v>803</v>
+      </c>
+      <c r="C284" t="s">
         <v>804</v>
       </c>
-      <c r="C284" t="s">
+      <c r="D284" t="s">
         <v>805</v>
       </c>
-      <c r="D284" t="s">
-        <v>806</v>
-      </c>
       <c r="E284">
         <v>0</v>
       </c>
@@ -9753,19 +9753,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>284</v>
       </c>
       <c r="B285" t="s">
+        <v>806</v>
+      </c>
+      <c r="C285" t="s">
         <v>807</v>
       </c>
-      <c r="C285" t="s">
+      <c r="D285" t="s">
         <v>808</v>
       </c>
-      <c r="D285" t="s">
-        <v>809</v>
-      </c>
       <c r="E285">
         <v>0</v>
       </c>
@@ -9773,19 +9773,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>285</v>
       </c>
       <c r="B286" t="s">
+        <v>809</v>
+      </c>
+      <c r="C286" t="s">
         <v>810</v>
       </c>
-      <c r="C286" t="s">
+      <c r="D286" t="s">
         <v>811</v>
       </c>
-      <c r="D286" t="s">
-        <v>812</v>
-      </c>
       <c r="E286">
         <v>0</v>
       </c>
@@ -9793,19 +9793,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>286</v>
       </c>
       <c r="B287" t="s">
+        <v>812</v>
+      </c>
+      <c r="C287" t="s">
         <v>813</v>
       </c>
-      <c r="C287" t="s">
+      <c r="D287" t="s">
         <v>814</v>
       </c>
-      <c r="D287" t="s">
-        <v>815</v>
-      </c>
       <c r="E287">
         <v>0</v>
       </c>
@@ -9813,15 +9813,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>287</v>
       </c>
       <c r="B288" t="s">
+        <v>815</v>
+      </c>
+      <c r="C288" t="s">
         <v>816</v>
-      </c>
-      <c r="C288" t="s">
-        <v>817</v>
       </c>
       <c r="D288" t="s">
         <v>481</v>
@@ -9833,19 +9833,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>288</v>
       </c>
       <c r="B289" t="s">
+        <v>817</v>
+      </c>
+      <c r="C289" t="s">
         <v>818</v>
       </c>
-      <c r="C289" t="s">
+      <c r="D289" t="s">
         <v>819</v>
       </c>
-      <c r="D289" t="s">
-        <v>820</v>
-      </c>
       <c r="E289">
         <v>0</v>
       </c>
@@ -9853,19 +9853,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>289</v>
       </c>
       <c r="B290" t="s">
+        <v>820</v>
+      </c>
+      <c r="C290" t="s">
         <v>821</v>
       </c>
-      <c r="C290" t="s">
+      <c r="D290" t="s">
         <v>822</v>
       </c>
-      <c r="D290" t="s">
-        <v>823</v>
-      </c>
       <c r="E290">
         <v>0</v>
       </c>
@@ -9873,19 +9873,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>290</v>
       </c>
       <c r="B291" t="s">
+        <v>823</v>
+      </c>
+      <c r="C291" t="s">
         <v>824</v>
       </c>
-      <c r="C291" t="s">
+      <c r="D291" t="s">
         <v>825</v>
       </c>
-      <c r="D291" t="s">
-        <v>826</v>
-      </c>
       <c r="E291">
         <v>0</v>
       </c>
@@ -9893,19 +9893,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>291</v>
       </c>
       <c r="B292" t="s">
+        <v>826</v>
+      </c>
+      <c r="C292" t="s">
         <v>827</v>
       </c>
-      <c r="C292" t="s">
+      <c r="D292" t="s">
         <v>828</v>
       </c>
-      <c r="D292" t="s">
-        <v>829</v>
-      </c>
       <c r="E292">
         <v>0</v>
       </c>
@@ -9913,19 +9913,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>292</v>
       </c>
       <c r="B293" t="s">
+        <v>829</v>
+      </c>
+      <c r="C293" t="s">
         <v>830</v>
       </c>
-      <c r="C293" t="s">
+      <c r="D293" t="s">
         <v>831</v>
       </c>
-      <c r="D293" t="s">
-        <v>832</v>
-      </c>
       <c r="E293">
         <v>0</v>
       </c>
@@ -9933,19 +9933,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>293</v>
       </c>
       <c r="B294" t="s">
+        <v>832</v>
+      </c>
+      <c r="C294" t="s">
         <v>833</v>
       </c>
-      <c r="C294" t="s">
+      <c r="D294" t="s">
         <v>834</v>
       </c>
-      <c r="D294" t="s">
-        <v>835</v>
-      </c>
       <c r="E294">
         <v>0</v>
       </c>
@@ -9953,19 +9953,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>294</v>
       </c>
       <c r="B295" t="s">
+        <v>835</v>
+      </c>
+      <c r="C295" t="s">
         <v>836</v>
       </c>
-      <c r="C295" t="s">
+      <c r="D295" t="s">
         <v>837</v>
       </c>
-      <c r="D295" t="s">
-        <v>838</v>
-      </c>
       <c r="E295">
         <v>0</v>
       </c>
@@ -9973,19 +9973,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>295</v>
       </c>
       <c r="B296" t="s">
+        <v>838</v>
+      </c>
+      <c r="C296" t="s">
         <v>839</v>
       </c>
-      <c r="C296" t="s">
+      <c r="D296" t="s">
         <v>840</v>
       </c>
-      <c r="D296" t="s">
-        <v>841</v>
-      </c>
       <c r="E296">
         <v>0</v>
       </c>
@@ -9993,19 +9993,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>296</v>
       </c>
       <c r="B297" t="s">
+        <v>841</v>
+      </c>
+      <c r="C297" t="s">
         <v>842</v>
       </c>
-      <c r="C297" t="s">
+      <c r="D297" t="s">
         <v>843</v>
       </c>
-      <c r="D297" t="s">
-        <v>844</v>
-      </c>
       <c r="E297">
         <v>0</v>
       </c>
@@ -10013,19 +10013,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>297</v>
       </c>
       <c r="B298" t="s">
+        <v>844</v>
+      </c>
+      <c r="C298" t="s">
         <v>845</v>
       </c>
-      <c r="C298" t="s">
+      <c r="D298" t="s">
         <v>846</v>
       </c>
-      <c r="D298" t="s">
-        <v>847</v>
-      </c>
       <c r="E298">
         <v>0</v>
       </c>
@@ -10033,15 +10033,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>298</v>
       </c>
       <c r="B299" t="s">
+        <v>847</v>
+      </c>
+      <c r="C299" t="s">
         <v>848</v>
-      </c>
-      <c r="C299" t="s">
-        <v>849</v>
       </c>
       <c r="D299" t="s">
         <v>254</v>
@@ -10053,19 +10053,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>299</v>
       </c>
       <c r="B300" t="s">
+        <v>849</v>
+      </c>
+      <c r="C300" t="s">
         <v>850</v>
       </c>
-      <c r="C300" t="s">
+      <c r="D300" t="s">
         <v>851</v>
       </c>
-      <c r="D300" t="s">
-        <v>852</v>
-      </c>
       <c r="E300">
         <v>0</v>
       </c>
@@ -10073,19 +10073,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>300</v>
       </c>
       <c r="B301" t="s">
+        <v>852</v>
+      </c>
+      <c r="C301" t="s">
         <v>853</v>
       </c>
-      <c r="C301" t="s">
+      <c r="D301" t="s">
         <v>854</v>
       </c>
-      <c r="D301" t="s">
-        <v>855</v>
-      </c>
       <c r="E301">
         <v>0</v>
       </c>
@@ -10093,19 +10093,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>301</v>
       </c>
       <c r="B302" t="s">
+        <v>855</v>
+      </c>
+      <c r="C302" t="s">
         <v>856</v>
       </c>
-      <c r="C302" t="s">
+      <c r="D302" t="s">
         <v>857</v>
       </c>
-      <c r="D302" t="s">
-        <v>858</v>
-      </c>
       <c r="E302">
         <v>0</v>
       </c>
@@ -10113,19 +10113,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>302</v>
       </c>
       <c r="B303" t="s">
+        <v>858</v>
+      </c>
+      <c r="C303" t="s">
         <v>859</v>
       </c>
-      <c r="C303" t="s">
+      <c r="D303" t="s">
         <v>860</v>
       </c>
-      <c r="D303" t="s">
-        <v>861</v>
-      </c>
       <c r="E303">
         <v>0</v>
       </c>
@@ -10133,19 +10133,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>303</v>
       </c>
       <c r="B304" t="s">
+        <v>861</v>
+      </c>
+      <c r="C304" t="s">
         <v>862</v>
       </c>
-      <c r="C304" t="s">
+      <c r="D304" t="s">
         <v>863</v>
       </c>
-      <c r="D304" t="s">
-        <v>864</v>
-      </c>
       <c r="E304">
         <v>0</v>
       </c>
@@ -10153,19 +10153,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>304</v>
       </c>
       <c r="B305" t="s">
+        <v>864</v>
+      </c>
+      <c r="C305" t="s">
         <v>865</v>
       </c>
-      <c r="C305" t="s">
+      <c r="D305" t="s">
         <v>866</v>
       </c>
-      <c r="D305" t="s">
-        <v>867</v>
-      </c>
       <c r="E305">
         <v>0</v>
       </c>
@@ -10173,19 +10173,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>305</v>
       </c>
       <c r="B306" t="s">
+        <v>867</v>
+      </c>
+      <c r="C306" t="s">
         <v>868</v>
       </c>
-      <c r="C306" t="s">
+      <c r="D306" t="s">
         <v>869</v>
       </c>
-      <c r="D306" t="s">
-        <v>870</v>
-      </c>
       <c r="E306">
         <v>0</v>
       </c>
@@ -10193,15 +10193,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>306</v>
       </c>
       <c r="B307" t="s">
+        <v>870</v>
+      </c>
+      <c r="C307" t="s">
         <v>871</v>
-      </c>
-      <c r="C307" t="s">
-        <v>872</v>
       </c>
       <c r="D307" t="s">
         <v>254</v>
@@ -10213,7 +10213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>307</v>
       </c>
@@ -10221,11 +10221,11 @@
         <v>148</v>
       </c>
       <c r="C308" t="s">
+        <v>872</v>
+      </c>
+      <c r="D308" t="s">
         <v>873</v>
       </c>
-      <c r="D308" t="s">
-        <v>874</v>
-      </c>
       <c r="E308">
         <v>0</v>
       </c>
@@ -10233,19 +10233,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>308</v>
       </c>
       <c r="B309" t="s">
+        <v>874</v>
+      </c>
+      <c r="C309" t="s">
         <v>875</v>
       </c>
-      <c r="C309" t="s">
+      <c r="D309" t="s">
         <v>876</v>
       </c>
-      <c r="D309" t="s">
-        <v>877</v>
-      </c>
       <c r="E309">
         <v>0</v>
       </c>
@@ -10253,19 +10253,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>309</v>
       </c>
       <c r="B310" t="s">
+        <v>877</v>
+      </c>
+      <c r="C310" t="s">
         <v>878</v>
       </c>
-      <c r="C310" t="s">
+      <c r="D310" t="s">
         <v>879</v>
       </c>
-      <c r="D310" t="s">
-        <v>880</v>
-      </c>
       <c r="E310">
         <v>0</v>
       </c>
@@ -10273,19 +10273,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>310</v>
       </c>
       <c r="B311" t="s">
+        <v>880</v>
+      </c>
+      <c r="C311" t="s">
         <v>881</v>
       </c>
-      <c r="C311" t="s">
+      <c r="D311" t="s">
         <v>882</v>
       </c>
-      <c r="D311" t="s">
-        <v>883</v>
-      </c>
       <c r="E311">
         <v>0</v>
       </c>
@@ -10293,19 +10293,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>311</v>
       </c>
       <c r="B312" t="s">
+        <v>883</v>
+      </c>
+      <c r="C312" t="s">
         <v>884</v>
       </c>
-      <c r="C312" t="s">
+      <c r="D312" t="s">
         <v>885</v>
       </c>
-      <c r="D312" t="s">
-        <v>886</v>
-      </c>
       <c r="E312">
         <v>0</v>
       </c>
@@ -10313,15 +10313,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>312</v>
       </c>
       <c r="B313" t="s">
+        <v>886</v>
+      </c>
+      <c r="C313" t="s">
         <v>887</v>
-      </c>
-      <c r="C313" t="s">
-        <v>888</v>
       </c>
       <c r="D313" t="s">
         <v>189</v>
@@ -10333,19 +10333,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>313</v>
       </c>
       <c r="B314" t="s">
+        <v>888</v>
+      </c>
+      <c r="C314" t="s">
         <v>889</v>
       </c>
-      <c r="C314" t="s">
+      <c r="D314" t="s">
         <v>890</v>
       </c>
-      <c r="D314" t="s">
-        <v>891</v>
-      </c>
       <c r="E314">
         <v>0</v>
       </c>
@@ -10353,19 +10353,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>314</v>
       </c>
       <c r="B315" t="s">
+        <v>891</v>
+      </c>
+      <c r="C315" t="s">
         <v>892</v>
       </c>
-      <c r="C315" t="s">
+      <c r="D315" t="s">
         <v>893</v>
       </c>
-      <c r="D315" t="s">
-        <v>894</v>
-      </c>
       <c r="E315">
         <v>0</v>
       </c>
@@ -10373,18 +10373,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>315</v>
       </c>
       <c r="B316" t="s">
+        <v>894</v>
+      </c>
+      <c r="C316" t="s">
         <v>895</v>
       </c>
-      <c r="C316" t="s">
-        <v>896</v>
-      </c>
       <c r="D316" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E316">
         <v>0</v>

</xml_diff>